<commit_message>
Site updated: 2021-03-16 20:16:16
</commit_message>
<xml_diff>
--- a/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
+++ b/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\93497\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blog\source\post-images\A-Survey-on-Multi-Label-Data-Stream-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DCA9D7-AFC1-4FDD-9A37-943AAC5D03EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF907E7E-5DC4-49E3-9B50-E432C5ACE31F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
   <si>
     <t>算法</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>C:结构类</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>D:标签噪声</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,10 +139,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>F：高维度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>√</t>
   </si>
   <si>
@@ -207,6 +199,146 @@
   </si>
   <si>
     <t>LLSF学习类依赖标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C:结构化类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F：高维特征</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF-PCT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FaIE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEML</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LCML</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PLST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPLST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESMC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LNEMLC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预测聚类树的随机森林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特征感知的隐式标签空间编码</t>
+  </si>
+  <si>
+    <t>低等级经验风险最小化</t>
+  </si>
+  <si>
+    <t>标签相关性和缺少标签</t>
+  </si>
+  <si>
+    <t>主标签空间转换</t>
+  </si>
+  <si>
+    <t>条件主标签空间转换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高效的半监督多标签分类器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于多标签分类的标签网络嵌入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A：标签想关性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B：类不平衡性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C：类层次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:标签缺失</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E：高维特征</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENMLC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CBMLC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAkEL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LPLC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多标签分类集成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剪枝集合集成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基于聚类的方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>局部配对标签相关</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机k标签集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C：类稀疏行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D：标签缺失</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E：大规模标签</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -250,13 +382,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -557,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -606,10 +741,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -617,10 +752,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -628,13 +763,13 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -642,16 +777,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -659,13 +794,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -673,13 +808,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -687,10 +822,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -698,16 +833,16 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -715,13 +850,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,13 +864,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -743,10 +878,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,7 +889,7 @@
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -762,10 +897,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -773,10 +908,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,20 +922,369 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>27</v>
       </c>
-      <c r="G18" t="s">
-        <v>28</v>
-      </c>
       <c r="H18" t="s">
-        <v>29</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" t="s">
+        <v>29</v>
+      </c>
+      <c r="G45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" t="s">
+        <v>29</v>
+      </c>
+      <c r="G46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" t="s">
+        <v>78</v>
+      </c>
+      <c r="G48" t="s">
+        <v>79</v>
+      </c>
+      <c r="H48" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="13">
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>

</xml_diff>

<commit_message>
Site updated: 2021-03-17 17:48:23
</commit_message>
<xml_diff>
--- a/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
+++ b/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blog\source\post-images\A-Survey-on-Multi-Label-Data-Stream-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF907E7E-5DC4-49E3-9B50-E432C5ACE31F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAFFDB7-E4DA-4566-A95C-384735B0393A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="117">
   <si>
     <t>算法</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -339,6 +339,154 @@
   </si>
   <si>
     <t>E：大规模标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>训练复杂度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试复杂度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PT(问题转移)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AA（自适应算法）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ensemble（集成）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ML-kNN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ML-DT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CML</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rank-SVM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(q * F(m,d))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(q * F(m,d + q))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(q^2 * F(m,d))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(q^2 * F'(d))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(q * F'(d + q))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(q * F'(d))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片，视频，生物信息，文本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片，生物信息，文本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(m^2d + qmk)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(mdq)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(F(dq + q^2,m))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(md + qk)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(mq)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O((dq + q^2) * 2^q)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(n *  F(m,d,2^k))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(F(dq + mq^2,mq^2) + q^2(q + m))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(dq)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O(n * FM(d,2^k))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生物信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m:训练集的数量;d:维度；q:可能的类标签数量；k:k次；F(a,b) 和 F'(a,b)：某些方法的费用</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -382,16 +530,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,50 +824,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="41.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="28.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
@@ -935,37 +1089,37 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="3" t="s">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="1" t="s">
         <v>18</v>
       </c>
@@ -1122,38 +1276,38 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="3" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="1" t="s">
         <v>18</v>
       </c>
@@ -1275,8 +1429,184 @@
         <v>45</v>
       </c>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" t="s">
+        <v>99</v>
+      </c>
+      <c r="E54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" t="s">
+        <v>97</v>
+      </c>
+      <c r="D55" t="s">
+        <v>98</v>
+      </c>
+      <c r="E55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" t="s">
+        <v>106</v>
+      </c>
+      <c r="D58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="D59" t="s">
+        <v>99</v>
+      </c>
+      <c r="E59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" t="s">
+        <v>113</v>
+      </c>
+      <c r="E60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" t="s">
+        <v>111</v>
+      </c>
+      <c r="D61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:H40"/>
@@ -1285,11 +1615,6 @@
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Site updated: 2021-03-23 20:56:51
</commit_message>
<xml_diff>
--- a/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
+++ b/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blog\source\post-images\A-Survey-on-Multi-Label-Data-Stream-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAFFDB7-E4DA-4566-A95C-384735B0393A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F614E6-6D1C-4174-939B-CFE142DF10EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="167">
   <si>
     <t>算法</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -487,6 +487,195 @@
   </si>
   <si>
     <t>m:训练集的数量;d:维度；q:可能的类标签数量；k:k次；F(a,b) 和 F'(a,b)：某些方法的费用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>LC(D)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情感</t>
+  </si>
+  <si>
+    <t>情境</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>酵母</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>医学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>安然公司邮件数据集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Core15k</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tmc2007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mediamill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delicious</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>媒体</t>
+  </si>
+  <si>
+    <t>媒体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文本</t>
+  </si>
+  <si>
+    <t>tR：训练样本的数目；tN测试样本的数目；M：特征数目；L标签的数量；LC（D）：标签基数</t>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nursery</t>
+  </si>
+  <si>
+    <t>Adult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Census-Income</t>
+  </si>
+  <si>
+    <t>Forest coverage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yahoo Shopping</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electricity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KDDCup99</t>
+  </si>
+  <si>
+    <t>N:实例的数量；M：特征的数量；L：类标签的数量</t>
+  </si>
+  <si>
+    <t>113k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ensemble</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSML-ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dw-ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RLS-Multi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MuENL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iSOUP-Tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据流的SML-ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多标签数据流的dw-ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为了不平衡数据流</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于概念演化</t>
+  </si>
+  <si>
+    <t>MOA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据流学习框架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类回归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C：大量类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E：新的或重复的类</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -530,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -539,10 +728,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -824,53 +1023,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:E62"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="28.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
@@ -1089,37 +1288,37 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
       <c r="G26" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="1" t="s">
         <v>18</v>
       </c>
@@ -1276,38 +1475,38 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3" t="s">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
       <c r="H41" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="1" t="s">
         <v>18</v>
       </c>
@@ -1447,7 +1646,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B53" t="s">
@@ -1464,7 +1663,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+      <c r="A54" s="8"/>
       <c r="B54" t="s">
         <v>89</v>
       </c>
@@ -1479,7 +1678,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="8"/>
       <c r="B55" t="s">
         <v>90</v>
       </c>
@@ -1494,7 +1693,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B56" t="s">
@@ -1511,7 +1710,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
+      <c r="A57" s="8"/>
       <c r="B57" t="s">
         <v>92</v>
       </c>
@@ -1526,7 +1725,7 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
+      <c r="A58" s="8"/>
       <c r="B58" t="s">
         <v>93</v>
       </c>
@@ -1541,7 +1740,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="8" t="s">
         <v>87</v>
       </c>
       <c r="B59" t="s">
@@ -1558,7 +1757,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
+      <c r="A60" s="8"/>
       <c r="B60" t="s">
         <v>70</v>
       </c>
@@ -1573,7 +1772,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
+      <c r="A61" s="8"/>
       <c r="B61" t="s">
         <v>94</v>
       </c>
@@ -1588,33 +1787,596 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" t="s">
+        <v>118</v>
+      </c>
+      <c r="C72" t="s">
+        <v>119</v>
+      </c>
+      <c r="D72" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F72" t="s">
+        <v>122</v>
+      </c>
+      <c r="G72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>124</v>
+      </c>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73">
+        <v>391</v>
+      </c>
+      <c r="D73">
+        <v>202</v>
+      </c>
+      <c r="E73">
+        <v>72</v>
+      </c>
+      <c r="F73">
+        <v>6</v>
+      </c>
+      <c r="G73">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>125</v>
+      </c>
+      <c r="B74" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74">
+        <v>1211</v>
+      </c>
+      <c r="D74">
+        <v>1159</v>
+      </c>
+      <c r="E74">
+        <v>294</v>
+      </c>
+      <c r="F74">
+        <v>6</v>
+      </c>
+      <c r="G74">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>126</v>
+      </c>
+      <c r="B75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75">
+        <v>1500</v>
+      </c>
+      <c r="D75">
+        <v>917</v>
+      </c>
+      <c r="E75">
+        <v>103</v>
+      </c>
+      <c r="F75">
+        <v>14</v>
+      </c>
+      <c r="G75">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>127</v>
+      </c>
+      <c r="B76" t="s">
+        <v>115</v>
+      </c>
+      <c r="C76">
+        <v>645</v>
+      </c>
+      <c r="D76">
+        <v>333</v>
+      </c>
+      <c r="E76">
+        <v>1449</v>
+      </c>
+      <c r="F76">
+        <v>45</v>
+      </c>
+      <c r="G76">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>128</v>
+      </c>
+      <c r="B77" t="s">
+        <v>136</v>
+      </c>
+      <c r="C77">
+        <v>1123</v>
+      </c>
+      <c r="D77">
+        <v>579</v>
+      </c>
+      <c r="E77">
+        <v>1001</v>
+      </c>
+      <c r="F77">
+        <v>53</v>
+      </c>
+      <c r="G77">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>129</v>
+      </c>
+      <c r="B78" t="s">
+        <v>133</v>
+      </c>
+      <c r="C78">
+        <v>4500</v>
+      </c>
+      <c r="D78">
+        <v>500</v>
+      </c>
+      <c r="E78">
+        <v>499</v>
+      </c>
+      <c r="F78">
+        <v>374</v>
+      </c>
+      <c r="G78">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>130</v>
+      </c>
+      <c r="B79" t="s">
+        <v>136</v>
+      </c>
+      <c r="C79">
+        <v>21519</v>
+      </c>
+      <c r="D79">
+        <v>7077</v>
+      </c>
+      <c r="E79">
+        <v>500</v>
+      </c>
+      <c r="F79">
+        <v>22</v>
+      </c>
+      <c r="G79">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>131</v>
+      </c>
+      <c r="B80" t="s">
+        <v>133</v>
+      </c>
+      <c r="C80">
+        <v>30993</v>
+      </c>
+      <c r="D80">
+        <v>12914</v>
+      </c>
+      <c r="E80">
+        <v>120</v>
+      </c>
+      <c r="F80">
+        <v>101</v>
+      </c>
+      <c r="G80">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>132</v>
+      </c>
+      <c r="B81" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81">
+        <v>12920</v>
+      </c>
+      <c r="D81">
+        <v>3185</v>
+      </c>
+      <c r="E81">
+        <v>500</v>
+      </c>
+      <c r="F81">
+        <v>983</v>
+      </c>
+      <c r="G81">
+        <v>19.02</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89" t="s">
+        <v>121</v>
+      </c>
+      <c r="D89" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>143</v>
+      </c>
+      <c r="B90" s="4">
+        <v>581000</v>
+      </c>
+      <c r="C90">
+        <v>54</v>
+      </c>
+      <c r="D90">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" s="4">
+        <v>12960</v>
+      </c>
+      <c r="C91">
+        <v>8</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>141</v>
+      </c>
+      <c r="B92" s="4">
+        <v>48842</v>
+      </c>
+      <c r="C92">
+        <v>14</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>141</v>
+      </c>
+      <c r="B93" s="4">
+        <v>67557</v>
+      </c>
+      <c r="C93">
+        <v>41</v>
+      </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94" s="4">
+        <v>299285</v>
+      </c>
+      <c r="C94">
+        <v>40</v>
+      </c>
+      <c r="D94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>144</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C95">
+        <v>22</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>145</v>
+      </c>
+      <c r="B96" s="4">
+        <v>45312</v>
+      </c>
+      <c r="C96">
+        <v>7</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>146</v>
+      </c>
+      <c r="B97" s="4">
+        <v>490000</v>
+      </c>
+      <c r="C97">
+        <v>34</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E104" s="8"/>
+      <c r="F104" s="8"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="8"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E105" s="8"/>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="8"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B107" t="s">
+        <v>153</v>
+      </c>
+      <c r="C107" t="s">
+        <v>158</v>
+      </c>
+      <c r="E107" t="s">
+        <v>29</v>
+      </c>
+      <c r="I107" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="8"/>
+      <c r="B108" t="s">
+        <v>154</v>
+      </c>
+      <c r="C108" t="s">
+        <v>159</v>
+      </c>
+      <c r="E108" t="s">
+        <v>29</v>
+      </c>
+      <c r="F108" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="8"/>
+      <c r="B109" t="s">
+        <v>155</v>
+      </c>
+      <c r="C109" t="s">
+        <v>160</v>
+      </c>
+      <c r="E109" t="s">
+        <v>29</v>
+      </c>
+      <c r="G109" t="s">
+        <v>29</v>
+      </c>
+      <c r="I109" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B110" t="s">
+        <v>156</v>
+      </c>
+      <c r="C110" t="s">
+        <v>161</v>
+      </c>
+      <c r="D110" t="s">
+        <v>29</v>
+      </c>
+      <c r="F110" t="s">
+        <v>29</v>
+      </c>
+      <c r="H110" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B111" t="s">
+        <v>162</v>
+      </c>
+      <c r="C111" t="s">
+        <v>163</v>
+      </c>
+      <c r="E111" t="s">
+        <v>29</v>
+      </c>
+      <c r="F111" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="8"/>
+      <c r="B112" t="s">
+        <v>157</v>
+      </c>
+      <c r="C112" t="s">
+        <v>164</v>
+      </c>
+      <c r="E112" t="s">
+        <v>29</v>
+      </c>
+      <c r="F112" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>62</v>
+      </c>
+      <c r="E113" t="s">
+        <v>63</v>
+      </c>
+      <c r="F113" t="s">
+        <v>165</v>
+      </c>
+      <c r="G113" t="s">
+        <v>78</v>
+      </c>
+      <c r="H113" t="s">
+        <v>166</v>
+      </c>
+      <c r="I113" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:E62"/>
+  <mergeCells count="26">
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="B104:B106"/>
+    <mergeCell ref="C104:C106"/>
+    <mergeCell ref="D104:I104"/>
+    <mergeCell ref="D105:H105"/>
+    <mergeCell ref="A98:D98"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:E62"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:H40"/>
     <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Site updated: 2021-03-24 19:00:44
</commit_message>
<xml_diff>
--- a/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
+++ b/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blog\source\post-images\A-Survey-on-Multi-Label-Data-Stream-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F614E6-6D1C-4174-939B-CFE142DF10EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B42235-BC54-4CC6-96D6-BDAE4FE03F50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="212">
   <si>
     <t>算法</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -676,6 +676,186 @@
   </si>
   <si>
     <t>E：新的或重复的类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMOTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMOA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DWA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WOS-ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ESOS-ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEFMSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CILPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LGEMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HTPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMART</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRFA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLDE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWMEC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DWVE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GOOWE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMLCM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GOOWE-ML</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>概念漂移和倾斜分布</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不平衡和部分标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合成流框架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两个固定窗口和KNN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类不平衡学习的ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类不平衡和概念学习的ELM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基于标签和主动学习</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分类器频繁标签组合</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标签组和熵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>两种非稳定数据生成过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基于ELM的在线多标签分类器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PS 的多标签 Hoeffding 树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流式多标签随机树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态流随机森林</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多标签动态集成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>标签相关和特征依赖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基于 ML-kNN 的加权集成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加权投票集成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态加权投票</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空间在线加权集成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>转移到目标回归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多标签学习的GOOWE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C：概念漂移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:大量标签</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -719,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,6 +922,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,17 +1206,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H113" sqref="H113"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
     <col min="4" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1787,13 +1970,13 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -2026,15 +2209,15 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -2163,12 +2346,12 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="7"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
@@ -2329,7 +2512,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
         <v>62</v>
       </c>
@@ -2349,24 +2532,452 @@
         <v>45</v>
       </c>
     </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C116" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D116" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E116" s="8"/>
+      <c r="F116" s="8"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8"/>
+      <c r="I116" s="8"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H118" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I118" s="7"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B119" t="s">
+        <v>167</v>
+      </c>
+      <c r="C119" t="s">
+        <v>188</v>
+      </c>
+      <c r="D119" t="s">
+        <v>29</v>
+      </c>
+      <c r="E119" t="s">
+        <v>29</v>
+      </c>
+      <c r="F119" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="8"/>
+      <c r="B120" t="s">
+        <v>168</v>
+      </c>
+      <c r="C120" t="s">
+        <v>189</v>
+      </c>
+      <c r="E120" t="s">
+        <v>29</v>
+      </c>
+      <c r="F120" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="8"/>
+      <c r="B121" t="s">
+        <v>169</v>
+      </c>
+      <c r="C121" t="s">
+        <v>190</v>
+      </c>
+      <c r="D121" t="s">
+        <v>29</v>
+      </c>
+      <c r="F121" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="8"/>
+      <c r="B122" t="s">
+        <v>170</v>
+      </c>
+      <c r="C122" t="s">
+        <v>191</v>
+      </c>
+      <c r="E122" t="s">
+        <v>29</v>
+      </c>
+      <c r="F122" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="8"/>
+      <c r="B123" t="s">
+        <v>171</v>
+      </c>
+      <c r="C123" t="s">
+        <v>192</v>
+      </c>
+      <c r="E123" t="s">
+        <v>29</v>
+      </c>
+      <c r="F123" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="8"/>
+      <c r="B124" t="s">
+        <v>172</v>
+      </c>
+      <c r="C124" t="s">
+        <v>193</v>
+      </c>
+      <c r="E124" t="s">
+        <v>29</v>
+      </c>
+      <c r="F124" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="8"/>
+      <c r="B125" t="s">
+        <v>173</v>
+      </c>
+      <c r="C125" t="s">
+        <v>194</v>
+      </c>
+      <c r="D125" t="s">
+        <v>29</v>
+      </c>
+      <c r="E125" t="s">
+        <v>29</v>
+      </c>
+      <c r="F125" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="8"/>
+      <c r="B126" t="s">
+        <v>174</v>
+      </c>
+      <c r="C126" t="s">
+        <v>195</v>
+      </c>
+      <c r="D126" t="s">
+        <v>29</v>
+      </c>
+      <c r="F126" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="8"/>
+      <c r="B127" t="s">
+        <v>175</v>
+      </c>
+      <c r="C127" t="s">
+        <v>196</v>
+      </c>
+      <c r="D127" t="s">
+        <v>29</v>
+      </c>
+      <c r="F127" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="8"/>
+      <c r="B128" t="s">
+        <v>176</v>
+      </c>
+      <c r="C128" t="s">
+        <v>197</v>
+      </c>
+      <c r="E128" t="s">
+        <v>29</v>
+      </c>
+      <c r="F128" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A129" s="8"/>
+      <c r="B129" t="s">
+        <v>153</v>
+      </c>
+      <c r="C129" t="s">
+        <v>198</v>
+      </c>
+      <c r="E129" t="s">
+        <v>29</v>
+      </c>
+      <c r="F129" t="s">
+        <v>29</v>
+      </c>
+      <c r="H129" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B130" t="s">
+        <v>177</v>
+      </c>
+      <c r="C130" t="s">
+        <v>199</v>
+      </c>
+      <c r="D130" t="s">
+        <v>29</v>
+      </c>
+      <c r="F130" t="s">
+        <v>29</v>
+      </c>
+      <c r="G130" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A131" s="8"/>
+      <c r="B131" t="s">
+        <v>178</v>
+      </c>
+      <c r="C131" t="s">
+        <v>200</v>
+      </c>
+      <c r="F131" t="s">
+        <v>29</v>
+      </c>
+      <c r="G131" t="s">
+        <v>29</v>
+      </c>
+      <c r="H131" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="8"/>
+      <c r="B132" t="s">
+        <v>179</v>
+      </c>
+      <c r="C132" t="s">
+        <v>201</v>
+      </c>
+      <c r="F132" t="s">
+        <v>29</v>
+      </c>
+      <c r="G132" t="s">
+        <v>29</v>
+      </c>
+      <c r="H132" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="8"/>
+      <c r="B133" t="s">
+        <v>180</v>
+      </c>
+      <c r="C133" t="s">
+        <v>202</v>
+      </c>
+      <c r="D133" t="s">
+        <v>29</v>
+      </c>
+      <c r="E133" t="s">
+        <v>29</v>
+      </c>
+      <c r="F133" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="8"/>
+      <c r="B134" t="s">
+        <v>181</v>
+      </c>
+      <c r="C134" t="s">
+        <v>203</v>
+      </c>
+      <c r="D134" t="s">
+        <v>29</v>
+      </c>
+      <c r="E134" t="s">
+        <v>29</v>
+      </c>
+      <c r="F134" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="8"/>
+      <c r="B135" t="s">
+        <v>182</v>
+      </c>
+      <c r="C135" t="s">
+        <v>204</v>
+      </c>
+      <c r="E135" t="s">
+        <v>29</v>
+      </c>
+      <c r="F135" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B136" t="s">
+        <v>183</v>
+      </c>
+      <c r="C136" t="s">
+        <v>205</v>
+      </c>
+      <c r="F136" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="8"/>
+      <c r="B137" t="s">
+        <v>184</v>
+      </c>
+      <c r="C137" t="s">
+        <v>206</v>
+      </c>
+      <c r="D137" t="s">
+        <v>29</v>
+      </c>
+      <c r="F137" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" s="8"/>
+      <c r="B138" t="s">
+        <v>185</v>
+      </c>
+      <c r="C138" t="s">
+        <v>207</v>
+      </c>
+      <c r="D138" t="s">
+        <v>29</v>
+      </c>
+      <c r="F138" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A139" s="8"/>
+      <c r="B139" t="s">
+        <v>186</v>
+      </c>
+      <c r="C139" t="s">
+        <v>208</v>
+      </c>
+      <c r="F139" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="8"/>
+      <c r="B140" t="s">
+        <v>187</v>
+      </c>
+      <c r="C140" t="s">
+        <v>209</v>
+      </c>
+      <c r="D140" t="s">
+        <v>29</v>
+      </c>
+      <c r="F140" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
+        <v>62</v>
+      </c>
+      <c r="E141" t="s">
+        <v>63</v>
+      </c>
+      <c r="F141" t="s">
+        <v>210</v>
+      </c>
+      <c r="G141" t="s">
+        <v>211</v>
+      </c>
+      <c r="H141" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
+  <mergeCells count="34">
+    <mergeCell ref="A119:A129"/>
+    <mergeCell ref="A130:A135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="D116:I116"/>
+    <mergeCell ref="D117:G117"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
     <mergeCell ref="C25:H25"/>
     <mergeCell ref="B104:B106"/>
     <mergeCell ref="C104:C106"/>
     <mergeCell ref="D104:I104"/>
     <mergeCell ref="D105:H105"/>
     <mergeCell ref="A98:D98"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="A82:G82"/>
     <mergeCell ref="A53:A55"/>
@@ -2377,6 +2988,11 @@
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:H40"/>
     <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Site updated: 2021-03-25 17:47:40
</commit_message>
<xml_diff>
--- a/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
+++ b/post-images/A-Survey-on-Multi-Label-Data-Stream-Classification/A Survey on Multi-Label Data Stream Classification_表格翻译.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blog\source\post-images\A-Survey-on-Multi-Label-Data-Stream-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B42235-BC54-4CC6-96D6-BDAE4FE03F50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5614BD-542E-4467-A989-1C2CC962DDE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="229">
   <si>
     <t>算法</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -856,6 +856,67 @@
   </si>
   <si>
     <t>D:大量标签</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">L </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LD(D)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MediaMill</t>
+  </si>
+  <si>
+    <t>TMC2007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rcv1-v2</t>
+  </si>
+  <si>
+    <t>IMDB</t>
+  </si>
+  <si>
+    <t>20NG</t>
+  </si>
+  <si>
+    <t>Ohsumed</t>
+  </si>
+  <si>
+    <t>Slashdot</t>
+  </si>
+  <si>
+    <t>Enron</t>
+  </si>
+  <si>
+    <t>视频</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yeast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reuters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Core15K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多媒体</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1206,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2957,13 +3018,343 @@
         <v>66</v>
       </c>
     </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>117</v>
+      </c>
+      <c r="B145" t="s">
+        <v>118</v>
+      </c>
+      <c r="C145" t="s">
+        <v>138</v>
+      </c>
+      <c r="D145" t="s">
+        <v>121</v>
+      </c>
+      <c r="E145" t="s">
+        <v>212</v>
+      </c>
+      <c r="F145" t="s">
+        <v>123</v>
+      </c>
+      <c r="G145" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>214</v>
+      </c>
+      <c r="B146" t="s">
+        <v>222</v>
+      </c>
+      <c r="C146">
+        <v>43907</v>
+      </c>
+      <c r="D146">
+        <v>120</v>
+      </c>
+      <c r="E146">
+        <v>101</v>
+      </c>
+      <c r="F146">
+        <v>4.3760000000000003</v>
+      </c>
+      <c r="G146">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>215</v>
+      </c>
+      <c r="B147" t="s">
+        <v>115</v>
+      </c>
+      <c r="C147">
+        <v>28596</v>
+      </c>
+      <c r="D147">
+        <v>500</v>
+      </c>
+      <c r="E147">
+        <v>22</v>
+      </c>
+      <c r="F147">
+        <v>2.16</v>
+      </c>
+      <c r="G147">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>216</v>
+      </c>
+      <c r="B148" t="s">
+        <v>115</v>
+      </c>
+      <c r="C148">
+        <v>804414</v>
+      </c>
+      <c r="D148">
+        <v>500</v>
+      </c>
+      <c r="E148">
+        <v>103</v>
+      </c>
+      <c r="F148">
+        <v>3.24</v>
+      </c>
+      <c r="G148">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>217</v>
+      </c>
+      <c r="B149" t="s">
+        <v>115</v>
+      </c>
+      <c r="C149">
+        <v>120919</v>
+      </c>
+      <c r="D149">
+        <v>1001</v>
+      </c>
+      <c r="E149">
+        <v>28</v>
+      </c>
+      <c r="F149">
+        <v>2</v>
+      </c>
+      <c r="G149">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>218</v>
+      </c>
+      <c r="B150" t="s">
+        <v>115</v>
+      </c>
+      <c r="C150">
+        <v>19300</v>
+      </c>
+      <c r="D150">
+        <v>1006</v>
+      </c>
+      <c r="E150">
+        <v>20</v>
+      </c>
+      <c r="F150">
+        <v>1.02</v>
+      </c>
+      <c r="G150">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>223</v>
+      </c>
+      <c r="B151" t="s">
+        <v>135</v>
+      </c>
+      <c r="C151">
+        <v>2417</v>
+      </c>
+      <c r="D151">
+        <v>103</v>
+      </c>
+      <c r="E151">
+        <v>14</v>
+      </c>
+      <c r="F151">
+        <v>4.2370000000000001</v>
+      </c>
+      <c r="G151">
+        <v>0.30299999999999999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>219</v>
+      </c>
+      <c r="B152" t="s">
+        <v>115</v>
+      </c>
+      <c r="C152">
+        <v>13529</v>
+      </c>
+      <c r="D152">
+        <v>1002</v>
+      </c>
+      <c r="E152">
+        <v>23</v>
+      </c>
+      <c r="F152">
+        <v>1.66</v>
+      </c>
+      <c r="G152">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>220</v>
+      </c>
+      <c r="B153" t="s">
+        <v>115</v>
+      </c>
+      <c r="C153">
+        <v>3782</v>
+      </c>
+      <c r="D153">
+        <v>1079</v>
+      </c>
+      <c r="E153">
+        <v>22</v>
+      </c>
+      <c r="F153">
+        <v>1.18</v>
+      </c>
+      <c r="G153">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>224</v>
+      </c>
+      <c r="B154" t="s">
+        <v>115</v>
+      </c>
+      <c r="C154">
+        <v>6000</v>
+      </c>
+      <c r="D154">
+        <v>500</v>
+      </c>
+      <c r="E154">
+        <v>101</v>
+      </c>
+      <c r="F154">
+        <v>2.88</v>
+      </c>
+      <c r="G154">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>221</v>
+      </c>
+      <c r="B155" t="s">
+        <v>115</v>
+      </c>
+      <c r="C155">
+        <v>1702</v>
+      </c>
+      <c r="D155">
+        <v>1001</v>
+      </c>
+      <c r="E155">
+        <v>53</v>
+      </c>
+      <c r="F155">
+        <v>3.4</v>
+      </c>
+      <c r="G155">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>225</v>
+      </c>
+      <c r="B156" t="s">
+        <v>101</v>
+      </c>
+      <c r="C156">
+        <v>2407</v>
+      </c>
+      <c r="D156">
+        <v>294</v>
+      </c>
+      <c r="E156">
+        <v>6</v>
+      </c>
+      <c r="F156">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="G156">
+        <v>0.17899999999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>226</v>
+      </c>
+      <c r="B157" t="s">
+        <v>115</v>
+      </c>
+      <c r="C157">
+        <v>978</v>
+      </c>
+      <c r="D157">
+        <v>1449</v>
+      </c>
+      <c r="E157">
+        <v>45</v>
+      </c>
+      <c r="F157">
+        <v>1.25</v>
+      </c>
+      <c r="G157">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>227</v>
+      </c>
+      <c r="B158" t="s">
+        <v>228</v>
+      </c>
+      <c r="C158">
+        <v>5000</v>
+      </c>
+      <c r="D158">
+        <v>499</v>
+      </c>
+      <c r="E158">
+        <v>374</v>
+      </c>
+      <c r="F158">
+        <v>3.52</v>
+      </c>
+      <c r="G158">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A119:A129"/>
-    <mergeCell ref="A130:A135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="B116:B118"/>
-    <mergeCell ref="C116:C118"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A104:A106"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:G41"/>
     <mergeCell ref="D116:I116"/>
     <mergeCell ref="D117:G117"/>
     <mergeCell ref="A116:A118"/>
@@ -2980,19 +3371,11 @@
     <mergeCell ref="A98:D98"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="A82:G82"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A104:A106"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A119:A129"/>
+    <mergeCell ref="A130:A135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="B116:B118"/>
+    <mergeCell ref="C116:C118"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>